<commit_message>
Excel file changed in Feature branch now
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somchaud\Downloads\selenium_project\selenium_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somchaud\Downloads\selenium_project\selenium_project\SeleniumProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA4CCFC8-341D-4F73-B078-DABD04B6506D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2D24AEA5-B659-4A7E-B59D-0E602707DACD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{BB326CAA-B99D-4E64-B2BF-542B25E53110}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>City</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Mar</t>
+  </si>
+  <si>
+    <t>Feature branch</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,6 +457,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
commit in feature 2 branch
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somchaud\Downloads\selenium_project\selenium_project\SeleniumProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8171A455-F575-414A-A559-C03762A769E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2C416C61-A411-4AE6-9271-882F6EC5D23C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{BB326CAA-B99D-4E64-B2BF-542B25E53110}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>City</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>Feature 2 file</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E09C5B1-4A1A-4DD5-AA74-9255392C65B0}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,6 +453,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>